<commit_message>
Update anomaly gating and regenerate outputs
</commit_message>
<xml_diff>
--- a/outputs/banks_components_analysis.xlsx
+++ b/outputs/banks_components_analysis.xlsx
@@ -541,15 +541,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CTG</t>
+          <t>VCB</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>28.62</v>
+        <v>38.66</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MINIMAL</t>
+          <t>LOW</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -558,13 +558,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>11.84</v>
+        <v>8.99</v>
       </c>
       <c r="F2" t="n">
-        <v>68.23</v>
+        <v>82.33</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -575,15 +575,15 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>VCB</t>
+          <t>CTG</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>27.97</v>
+        <v>37.04</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MINIMAL</t>
+          <t>LOW</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -592,13 +592,13 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>8.91</v>
+        <v>11.92</v>
       </c>
       <c r="F3" t="n">
-        <v>69.73</v>
+        <v>77.91</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -613,11 +613,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>27.7</v>
+        <v>36.38</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MINIMAL</t>
+          <t>LOW</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -626,13 +626,13 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>11.29</v>
+        <v>11.55</v>
       </c>
       <c r="F4" t="n">
-        <v>66.23999999999999</v>
+        <v>80.05</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -647,11 +647,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>27.67</v>
+        <v>35.72</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MINIMAL</t>
+          <t>LOW</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -660,13 +660,13 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>7.77</v>
+        <v>8.09</v>
       </c>
       <c r="F5" t="n">
-        <v>70.18000000000001</v>
+        <v>85.66</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -677,15 +677,15 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ACB</t>
+          <t>BIDV</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>27.31</v>
+        <v>34.48</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MINIMAL</t>
+          <t>LOW</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -694,13 +694,13 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>7.48</v>
+        <v>7.64</v>
       </c>
       <c r="F6" t="n">
-        <v>69.48</v>
+        <v>75.48999999999999</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -711,15 +711,15 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>EIB</t>
+          <t>STB</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>26.61</v>
+        <v>34.29</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MINIMAL</t>
+          <t>LOW</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -728,13 +728,13 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>7.28</v>
+        <v>9.92</v>
       </c>
       <c r="F7" t="n">
-        <v>67.69</v>
+        <v>72.36</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -745,15 +745,15 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>VPB</t>
+          <t>MBB</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>26.08</v>
+        <v>32.77</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MINIMAL</t>
+          <t>LOW</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -762,13 +762,13 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>6.49</v>
+        <v>8.710000000000001</v>
       </c>
       <c r="F8" t="n">
-        <v>67.08</v>
+        <v>76.53</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -779,30 +779,30 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MBB</t>
+          <t>VPB</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>25.66</v>
+        <v>32.61</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>MINIMAL</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>MINIMAL</t>
-        </is>
-      </c>
       <c r="E9" t="n">
-        <v>8.5</v>
+        <v>6.79</v>
       </c>
       <c r="F9" t="n">
-        <v>63.59</v>
+        <v>81.84999999999999</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -813,30 +813,30 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>STB</t>
+          <t>ACB</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>25.16</v>
+        <v>32.39</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>MINIMAL</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>MINIMAL</t>
-        </is>
-      </c>
       <c r="E10" t="n">
-        <v>9.5</v>
+        <v>7.77</v>
       </c>
       <c r="F10" t="n">
-        <v>61.04</v>
+        <v>80.09999999999999</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -847,27 +847,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BIDV</t>
+          <t>EIB</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>25.06</v>
+        <v>30.44</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>MINIMAL</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>MINIMAL</t>
-        </is>
-      </c>
       <c r="E11" t="n">
-        <v>7.35</v>
+        <v>7.24</v>
       </c>
       <c r="F11" t="n">
-        <v>63.21</v>
+        <v>78.7</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -940,22 +940,22 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>Very Low (7.5/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
+          <t>Very Low (7.8/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>High (69.5/100) - Liquidity Risk presents significant concerns requiring immediate attention and remediation.</t>
+          <t>Critical (80.1/100) - Liquidity Risk is at critical levels requiring urgent intervention and comprehensive action plan.</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>Very Low (0.0/100) - Anomaly Detection is well-managed with strong controls and minimal concerns.</t>
+          <t>Very Low (5.0/100) - Anomaly Detection is well-managed with strong controls and minimal concerns.</t>
         </is>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>ACB has an overall risk score of 27.3 classified as MINIMAL. The primary risk driver is Liquidity Risk (69.5), while Anomaly Risk (0.0) is the strongest performing area. The bank demonstrates strong risk management across all areas with minimal supervisory concerns.</t>
+          <t>ACB has an overall risk score of 32.4 classified as LOW. The primary risk driver is Liquidity Risk (80.1), while Anomaly Risk (5.0) is the strongest performing area. The bank shows generally sound practices but should address identified weaknesses proactively.</t>
         </is>
       </c>
     </row>
@@ -967,22 +967,22 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>Very Low (7.4/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
+          <t>Very Low (7.6/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>High (63.2/100) - Liquidity Risk presents significant concerns requiring immediate attention and remediation.</t>
+          <t>High (75.5/100) - Liquidity Risk presents significant concerns requiring immediate attention and remediation.</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>Very Low (0.0/100) - Anomaly Detection is well-managed with strong controls and minimal concerns.</t>
+          <t>Low (20.0/100) - Anomaly Detection is generally well-controlled with minor areas for improvement.</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>BIDV has an overall risk score of 25.1 classified as MINIMAL. The primary risk driver is Liquidity Risk (63.2), while Anomaly Risk (0.0) is the strongest performing area. The bank demonstrates strong risk management across all areas with minimal supervisory concerns.</t>
+          <t>BIDV has an overall risk score of 34.5 classified as LOW. The primary risk driver is Liquidity Risk (75.5), while Credit Risk (7.6) is the strongest performing area. The bank shows generally sound practices but should address identified weaknesses proactively.</t>
         </is>
       </c>
     </row>
@@ -994,22 +994,22 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>Very Low (11.8/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
+          <t>Very Low (11.9/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>High (68.2/100) - Liquidity Risk presents significant concerns requiring immediate attention and remediation.</t>
+          <t>High (77.9/100) - Liquidity Risk presents significant concerns requiring immediate attention and remediation.</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>Very Low (0.0/100) - Anomaly Detection is well-managed with strong controls and minimal concerns.</t>
+          <t>Low (20.0/100) - Anomaly Detection is generally well-controlled with minor areas for improvement.</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>CTG has an overall risk score of 28.6 classified as MINIMAL. The primary risk driver is Liquidity Risk (68.2), while Anomaly Risk (0.0) is the strongest performing area. The bank demonstrates strong risk management across all areas with minimal supervisory concerns.</t>
+          <t>CTG has an overall risk score of 37.0 classified as LOW. The primary risk driver is Liquidity Risk (77.9), while Credit Risk (11.9) is the strongest performing area. The bank shows generally sound practices but should address identified weaknesses proactively.</t>
         </is>
       </c>
     </row>
@@ -1021,12 +1021,12 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>Very Low (7.3/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
+          <t>Very Low (7.2/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>High (67.7/100) - Liquidity Risk presents significant concerns requiring immediate attention and remediation.</t>
+          <t>High (78.7/100) - Liquidity Risk presents significant concerns requiring immediate attention and remediation.</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>EIB has an overall risk score of 26.6 classified as MINIMAL. The primary risk driver is Liquidity Risk (67.7), while Anomaly Risk (0.0) is the strongest performing area. The bank demonstrates strong risk management across all areas with minimal supervisory concerns.</t>
+          <t>EIB has an overall risk score of 30.4 classified as LOW. The primary risk driver is Liquidity Risk (78.7), while Anomaly Risk (0.0) is the strongest performing area. The bank shows generally sound practices but should address identified weaknesses proactively.</t>
         </is>
       </c>
     </row>
@@ -1048,22 +1048,22 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>Very Low (11.3/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
+          <t>Very Low (11.5/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>High (66.2/100) - Liquidity Risk presents significant concerns requiring immediate attention and remediation.</t>
+          <t>Critical (80.0/100) - Liquidity Risk is at critical levels requiring urgent intervention and comprehensive action plan.</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>Very Low (0.0/100) - Anomaly Detection is well-managed with strong controls and minimal concerns.</t>
+          <t>Very Low (15.0/100) - Anomaly Detection is well-managed with strong controls and minimal concerns.</t>
         </is>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>HDB has an overall risk score of 27.7 classified as MINIMAL. The primary risk driver is Liquidity Risk (66.2), while Anomaly Risk (0.0) is the strongest performing area. The bank demonstrates strong risk management across all areas with minimal supervisory concerns.</t>
+          <t>HDB has an overall risk score of 36.4 classified as LOW. The primary risk driver is Liquidity Risk (80.0), while Credit Risk (11.5) is the strongest performing area. The bank shows generally sound practices but should address identified weaknesses proactively.</t>
         </is>
       </c>
     </row>
@@ -1075,22 +1075,22 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>Very Low (8.5/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
+          <t>Very Low (8.7/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>High (63.6/100) - Liquidity Risk presents significant concerns requiring immediate attention and remediation.</t>
+          <t>High (76.5/100) - Liquidity Risk presents significant concerns requiring immediate attention and remediation.</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
-          <t>Very Low (0.0/100) - Anomaly Detection is well-managed with strong controls and minimal concerns.</t>
+          <t>Very Low (10.0/100) - Anomaly Detection is well-managed with strong controls and minimal concerns.</t>
         </is>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>MBB has an overall risk score of 25.7 classified as MINIMAL. The primary risk driver is Liquidity Risk (63.6), while Anomaly Risk (0.0) is the strongest performing area. The bank demonstrates strong risk management across all areas with minimal supervisory concerns.</t>
+          <t>MBB has an overall risk score of 32.8 classified as LOW. The primary risk driver is Liquidity Risk (76.5), while Credit Risk (8.7) is the strongest performing area. The bank shows generally sound practices but should address identified weaknesses proactively.</t>
         </is>
       </c>
     </row>
@@ -1102,22 +1102,22 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>Very Low (9.5/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
+          <t>Very Low (9.9/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>High (61.0/100) - Liquidity Risk presents significant concerns requiring immediate attention and remediation.</t>
+          <t>High (72.4/100) - Liquidity Risk presents significant concerns requiring immediate attention and remediation.</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>Very Low (0.0/100) - Anomaly Detection is well-managed with strong controls and minimal concerns.</t>
+          <t>Low (20.0/100) - Anomaly Detection is generally well-controlled with minor areas for improvement.</t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>STB has an overall risk score of 25.2 classified as MINIMAL. The primary risk driver is Liquidity Risk (61.0), while Anomaly Risk (0.0) is the strongest performing area. The bank demonstrates strong risk management across all areas with minimal supervisory concerns.</t>
+          <t>STB has an overall risk score of 34.3 classified as LOW. The primary risk driver is Liquidity Risk (72.4), while Credit Risk (9.9) is the strongest performing area. The bank shows generally sound practices but should address identified weaknesses proactively.</t>
         </is>
       </c>
     </row>
@@ -1129,22 +1129,22 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Very Low (7.8/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
+          <t>Very Low (8.1/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>High (70.2/100) - Liquidity Risk presents significant concerns requiring immediate attention and remediation.</t>
+          <t>Critical (85.7/100) - Liquidity Risk is at critical levels requiring urgent intervention and comprehensive action plan.</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>Very Low (0.0/100) - Anomaly Detection is well-managed with strong controls and minimal concerns.</t>
+          <t>Very Low (10.0/100) - Anomaly Detection is well-managed with strong controls and minimal concerns.</t>
         </is>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>TCB has an overall risk score of 27.7 classified as MINIMAL. The primary risk driver is Liquidity Risk (70.2), while Anomaly Risk (0.0) is the strongest performing area. The bank demonstrates strong risk management across all areas with minimal supervisory concerns.</t>
+          <t>TCB has an overall risk score of 35.7 classified as LOW. The primary risk driver is Liquidity Risk (85.7), while Credit Risk (8.1) is the strongest performing area. The bank shows generally sound practices but should address identified weaknesses proactively.</t>
         </is>
       </c>
     </row>
@@ -1156,22 +1156,22 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>Very Low (8.9/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
+          <t>Very Low (9.0/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>High (69.7/100) - Liquidity Risk presents significant concerns requiring immediate attention and remediation.</t>
+          <t>Critical (82.3/100) - Liquidity Risk is at critical levels requiring urgent intervention and comprehensive action plan.</t>
         </is>
       </c>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>Very Low (0.0/100) - Anomaly Detection is well-managed with strong controls and minimal concerns.</t>
+          <t>Low (25.0/100) - Anomaly Detection is generally well-controlled with minor areas for improvement.</t>
         </is>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>VCB has an overall risk score of 28.0 classified as MINIMAL. The primary risk driver is Liquidity Risk (69.7), while Anomaly Risk (0.0) is the strongest performing area. The bank demonstrates strong risk management across all areas with minimal supervisory concerns.</t>
+          <t>VCB has an overall risk score of 38.7 classified as LOW. The primary risk driver is Liquidity Risk (82.3), while Credit Risk (9.0) is the strongest performing area. The bank shows generally sound practices but should address identified weaknesses proactively.</t>
         </is>
       </c>
     </row>
@@ -1183,22 +1183,22 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>Very Low (6.5/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
+          <t>Very Low (6.8/100) - Credit Risk is well-managed with strong controls and minimal concerns.</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>High (67.1/100) - Liquidity Risk presents significant concerns requiring immediate attention and remediation.</t>
+          <t>Critical (81.8/100) - Liquidity Risk is at critical levels requiring urgent intervention and comprehensive action plan.</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>Very Low (0.0/100) - Anomaly Detection is well-managed with strong controls and minimal concerns.</t>
+          <t>Very Low (5.0/100) - Anomaly Detection is well-managed with strong controls and minimal concerns.</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>VPB has an overall risk score of 26.1 classified as MINIMAL. The primary risk driver is Liquidity Risk (67.1), while Anomaly Risk (0.0) is the strongest performing area. The bank demonstrates strong risk management across all areas with minimal supervisory concerns.</t>
+          <t>VPB has an overall risk score of 32.6 classified as LOW. The primary risk driver is Liquidity Risk (81.8), while Anomaly Risk (5.0) is the strongest performing area. The bank shows generally sound practices but should address identified weaknesses proactively.</t>
         </is>
       </c>
     </row>
@@ -1265,551 +1265,551 @@
     <row r="2">
       <c r="A2" s="5" t="inlineStr">
         <is>
+          <t>ACB</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>Liquidity Risk</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>Critical liquidity concerns</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>Immediately improve liquidity position by increasing liquid assets, reducing loan-to-deposit ratio, and establishing contingency funding plans. Consider asset sales if necessary.</t>
+        </is>
+      </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>Immediate</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>BIDV</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>Liquidity Risk</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>Critical liquidity concerns</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>Immediately improve liquidity position by increasing liquid assets, reducing loan-to-deposit ratio, and establishing contingency funding plans. Consider asset sales if necessary.</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>Immediate</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>BIDV</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>Anomaly Detection</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>Significant anomalies detected</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>Conduct thorough investigation of all flagged transactions and activities. Enhance internal controls and fraud detection systems. Consider external audit.</t>
+        </is>
+      </c>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>7-14 days</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t>CTG</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>Liquidity Risk</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>Critical liquidity concerns</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>Immediately improve liquidity position by increasing liquid assets, reducing loan-to-deposit ratio, and establishing contingency funding plans. Consider asset sales if necessary.</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>Immediate</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>CTG</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>Anomaly Detection</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>Significant anomalies detected</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>Conduct thorough investigation of all flagged transactions and activities. Enhance internal controls and fraud detection systems. Consider external audit.</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>7-14 days</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>EIB</t>
+        </is>
+      </c>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>Liquidity Risk</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>Critical liquidity concerns</t>
+        </is>
+      </c>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>Immediately improve liquidity position by increasing liquid assets, reducing loan-to-deposit ratio, and establishing contingency funding plans. Consider asset sales if necessary.</t>
+        </is>
+      </c>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>Immediate</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>HDB</t>
+        </is>
+      </c>
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t>Liquidity Risk</t>
+        </is>
+      </c>
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>Critical liquidity concerns</t>
+        </is>
+      </c>
+      <c r="E8" s="5" t="inlineStr">
+        <is>
+          <t>Immediately improve liquidity position by increasing liquid assets, reducing loan-to-deposit ratio, and establishing contingency funding plans. Consider asset sales if necessary.</t>
+        </is>
+      </c>
+      <c r="F8" s="5" t="inlineStr">
+        <is>
+          <t>Immediate</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="inlineStr">
+        <is>
+          <t>HDB</t>
+        </is>
+      </c>
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t>Anomaly Detection</t>
+        </is>
+      </c>
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t>Significant anomalies detected</t>
+        </is>
+      </c>
+      <c r="E9" s="5" t="inlineStr">
+        <is>
+          <t>Conduct thorough investigation of all flagged transactions and activities. Enhance internal controls and fraud detection systems. Consider external audit.</t>
+        </is>
+      </c>
+      <c r="F9" s="5" t="inlineStr">
+        <is>
+          <t>7-14 days</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t>MBB</t>
+        </is>
+      </c>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>Liquidity Risk</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="inlineStr">
+        <is>
+          <t>Critical liquidity concerns</t>
+        </is>
+      </c>
+      <c r="E10" s="5" t="inlineStr">
+        <is>
+          <t>Immediately improve liquidity position by increasing liquid assets, reducing loan-to-deposit ratio, and establishing contingency funding plans. Consider asset sales if necessary.</t>
+        </is>
+      </c>
+      <c r="F10" s="5" t="inlineStr">
+        <is>
+          <t>Immediate</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="inlineStr">
+        <is>
+          <t>MBB</t>
+        </is>
+      </c>
+      <c r="B11" s="5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t>Anomaly Detection</t>
+        </is>
+      </c>
+      <c r="D11" s="5" t="inlineStr">
+        <is>
+          <t>Significant anomalies detected</t>
+        </is>
+      </c>
+      <c r="E11" s="5" t="inlineStr">
+        <is>
+          <t>Conduct thorough investigation of all flagged transactions and activities. Enhance internal controls and fraud detection systems. Consider external audit.</t>
+        </is>
+      </c>
+      <c r="F11" s="5" t="inlineStr">
+        <is>
+          <t>7-14 days</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>STB</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>Liquidity Risk</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="inlineStr">
+        <is>
+          <t>Critical liquidity concerns</t>
+        </is>
+      </c>
+      <c r="E12" s="5" t="inlineStr">
+        <is>
+          <t>Immediately improve liquidity position by increasing liquid assets, reducing loan-to-deposit ratio, and establishing contingency funding plans. Consider asset sales if necessary.</t>
+        </is>
+      </c>
+      <c r="F12" s="5" t="inlineStr">
+        <is>
+          <t>Immediate</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>STB</t>
+        </is>
+      </c>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>Anomaly Detection</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="inlineStr">
+        <is>
+          <t>Significant anomalies detected</t>
+        </is>
+      </c>
+      <c r="E13" s="5" t="inlineStr">
+        <is>
+          <t>Conduct thorough investigation of all flagged transactions and activities. Enhance internal controls and fraud detection systems. Consider external audit.</t>
+        </is>
+      </c>
+      <c r="F13" s="5" t="inlineStr">
+        <is>
+          <t>7-14 days</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="5" t="inlineStr">
+        <is>
           <t>TCB</t>
         </is>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B14" s="5" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C14" s="5" t="inlineStr">
         <is>
           <t>Liquidity Risk</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="D14" s="5" t="inlineStr">
         <is>
           <t>Critical liquidity concerns</t>
         </is>
       </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="E14" s="5" t="inlineStr">
         <is>
           <t>Immediately improve liquidity position by increasing liquid assets, reducing loan-to-deposit ratio, and establishing contingency funding plans. Consider asset sales if necessary.</t>
         </is>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="F14" s="5" t="inlineStr">
         <is>
           <t>Immediate</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>ACB</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>Credit Risk</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>Strong credit risk management</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>Continue existing practices. Share best practices with other institutions. Consider slight expansion within risk appetite.</t>
-        </is>
-      </c>
-      <c r="F3" s="3" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>ACB</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="inlineStr">
+    <row r="15">
+      <c r="A15" s="5" t="inlineStr">
+        <is>
+          <t>TCB</t>
+        </is>
+      </c>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
         <is>
           <t>Anomaly Detection</t>
         </is>
       </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>No significant anomalies</t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>Continue robust monitoring and detection systems. Regularly update detection algorithms and thresholds.</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>BIDV</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>Credit Risk</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>Strong credit risk management</t>
-        </is>
-      </c>
-      <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>Continue existing practices. Share best practices with other institutions. Consider slight expansion within risk appetite.</t>
-        </is>
-      </c>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>BIDV</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C6" s="3" t="inlineStr">
+      <c r="D15" s="5" t="inlineStr">
+        <is>
+          <t>Significant anomalies detected</t>
+        </is>
+      </c>
+      <c r="E15" s="5" t="inlineStr">
+        <is>
+          <t>Conduct thorough investigation of all flagged transactions and activities. Enhance internal controls and fraud detection systems. Consider external audit.</t>
+        </is>
+      </c>
+      <c r="F15" s="5" t="inlineStr">
+        <is>
+          <t>7-14 days</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="inlineStr">
+        <is>
+          <t>VCB</t>
+        </is>
+      </c>
+      <c r="B16" s="5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="C16" s="5" t="inlineStr">
+        <is>
+          <t>Liquidity Risk</t>
+        </is>
+      </c>
+      <c r="D16" s="5" t="inlineStr">
+        <is>
+          <t>Critical liquidity concerns</t>
+        </is>
+      </c>
+      <c r="E16" s="5" t="inlineStr">
+        <is>
+          <t>Immediately improve liquidity position by increasing liquid assets, reducing loan-to-deposit ratio, and establishing contingency funding plans. Consider asset sales if necessary.</t>
+        </is>
+      </c>
+      <c r="F16" s="5" t="inlineStr">
+        <is>
+          <t>Immediate</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="5" t="inlineStr">
+        <is>
+          <t>VCB</t>
+        </is>
+      </c>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
         <is>
           <t>Anomaly Detection</t>
         </is>
       </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>No significant anomalies</t>
-        </is>
-      </c>
-      <c r="E6" s="3" t="inlineStr">
-        <is>
-          <t>Continue robust monitoring and detection systems. Regularly update detection algorithms and thresholds.</t>
-        </is>
-      </c>
-      <c r="F6" s="3" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>CTG</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="inlineStr">
-        <is>
-          <t>Credit Risk</t>
-        </is>
-      </c>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>Strong credit risk management</t>
-        </is>
-      </c>
-      <c r="E7" s="3" t="inlineStr">
-        <is>
-          <t>Continue existing practices. Share best practices with other institutions. Consider slight expansion within risk appetite.</t>
-        </is>
-      </c>
-      <c r="F7" s="3" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="inlineStr">
-        <is>
-          <t>CTG</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C8" s="3" t="inlineStr">
-        <is>
-          <t>Anomaly Detection</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>No significant anomalies</t>
-        </is>
-      </c>
-      <c r="E8" s="3" t="inlineStr">
-        <is>
-          <t>Continue robust monitoring and detection systems. Regularly update detection algorithms and thresholds.</t>
-        </is>
-      </c>
-      <c r="F8" s="3" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="inlineStr">
-        <is>
-          <t>EIB</t>
-        </is>
-      </c>
-      <c r="B9" s="3" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C9" s="3" t="inlineStr">
-        <is>
-          <t>Credit Risk</t>
-        </is>
-      </c>
-      <c r="D9" s="3" t="inlineStr">
-        <is>
-          <t>Strong credit risk management</t>
-        </is>
-      </c>
-      <c r="E9" s="3" t="inlineStr">
-        <is>
-          <t>Continue existing practices. Share best practices with other institutions. Consider slight expansion within risk appetite.</t>
-        </is>
-      </c>
-      <c r="F9" s="3" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="inlineStr">
-        <is>
-          <t>EIB</t>
-        </is>
-      </c>
-      <c r="B10" s="3" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C10" s="3" t="inlineStr">
-        <is>
-          <t>Anomaly Detection</t>
-        </is>
-      </c>
-      <c r="D10" s="3" t="inlineStr">
-        <is>
-          <t>No significant anomalies</t>
-        </is>
-      </c>
-      <c r="E10" s="3" t="inlineStr">
-        <is>
-          <t>Continue robust monitoring and detection systems. Regularly update detection algorithms and thresholds.</t>
-        </is>
-      </c>
-      <c r="F10" s="3" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="inlineStr">
-        <is>
-          <t>HDB</t>
-        </is>
-      </c>
-      <c r="B11" s="3" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C11" s="3" t="inlineStr">
-        <is>
-          <t>Credit Risk</t>
-        </is>
-      </c>
-      <c r="D11" s="3" t="inlineStr">
-        <is>
-          <t>Strong credit risk management</t>
-        </is>
-      </c>
-      <c r="E11" s="3" t="inlineStr">
-        <is>
-          <t>Continue existing practices. Share best practices with other institutions. Consider slight expansion within risk appetite.</t>
-        </is>
-      </c>
-      <c r="F11" s="3" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="inlineStr">
-        <is>
-          <t>HDB</t>
-        </is>
-      </c>
-      <c r="B12" s="3" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C12" s="3" t="inlineStr">
-        <is>
-          <t>Anomaly Detection</t>
-        </is>
-      </c>
-      <c r="D12" s="3" t="inlineStr">
-        <is>
-          <t>No significant anomalies</t>
-        </is>
-      </c>
-      <c r="E12" s="3" t="inlineStr">
-        <is>
-          <t>Continue robust monitoring and detection systems. Regularly update detection algorithms and thresholds.</t>
-        </is>
-      </c>
-      <c r="F12" s="3" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="inlineStr">
-        <is>
-          <t>MBB</t>
-        </is>
-      </c>
-      <c r="B13" s="3" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C13" s="3" t="inlineStr">
-        <is>
-          <t>Credit Risk</t>
-        </is>
-      </c>
-      <c r="D13" s="3" t="inlineStr">
-        <is>
-          <t>Strong credit risk management</t>
-        </is>
-      </c>
-      <c r="E13" s="3" t="inlineStr">
-        <is>
-          <t>Continue existing practices. Share best practices with other institutions. Consider slight expansion within risk appetite.</t>
-        </is>
-      </c>
-      <c r="F13" s="3" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="3" t="inlineStr">
-        <is>
-          <t>MBB</t>
-        </is>
-      </c>
-      <c r="B14" s="3" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C14" s="3" t="inlineStr">
-        <is>
-          <t>Anomaly Detection</t>
-        </is>
-      </c>
-      <c r="D14" s="3" t="inlineStr">
-        <is>
-          <t>No significant anomalies</t>
-        </is>
-      </c>
-      <c r="E14" s="3" t="inlineStr">
-        <is>
-          <t>Continue robust monitoring and detection systems. Regularly update detection algorithms and thresholds.</t>
-        </is>
-      </c>
-      <c r="F14" s="3" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="3" t="inlineStr">
-        <is>
-          <t>STB</t>
-        </is>
-      </c>
-      <c r="B15" s="3" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C15" s="3" t="inlineStr">
-        <is>
-          <t>Credit Risk</t>
-        </is>
-      </c>
-      <c r="D15" s="3" t="inlineStr">
-        <is>
-          <t>Strong credit risk management</t>
-        </is>
-      </c>
-      <c r="E15" s="3" t="inlineStr">
-        <is>
-          <t>Continue existing practices. Share best practices with other institutions. Consider slight expansion within risk appetite.</t>
-        </is>
-      </c>
-      <c r="F15" s="3" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="3" t="inlineStr">
-        <is>
-          <t>STB</t>
-        </is>
-      </c>
-      <c r="B16" s="3" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C16" s="3" t="inlineStr">
-        <is>
-          <t>Anomaly Detection</t>
-        </is>
-      </c>
-      <c r="D16" s="3" t="inlineStr">
-        <is>
-          <t>No significant anomalies</t>
-        </is>
-      </c>
-      <c r="E16" s="3" t="inlineStr">
-        <is>
-          <t>Continue robust monitoring and detection systems. Regularly update detection algorithms and thresholds.</t>
-        </is>
-      </c>
-      <c r="F16" s="3" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="inlineStr">
-        <is>
-          <t>TCB</t>
-        </is>
-      </c>
-      <c r="B17" s="3" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C17" s="3" t="inlineStr">
-        <is>
-          <t>Credit Risk</t>
-        </is>
-      </c>
-      <c r="D17" s="3" t="inlineStr">
-        <is>
-          <t>Strong credit risk management</t>
-        </is>
-      </c>
-      <c r="E17" s="3" t="inlineStr">
-        <is>
-          <t>Continue existing practices. Share best practices with other institutions. Consider slight expansion within risk appetite.</t>
-        </is>
-      </c>
-      <c r="F17" s="3" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
+      <c r="D17" s="5" t="inlineStr">
+        <is>
+          <t>Significant anomalies detected</t>
+        </is>
+      </c>
+      <c r="E17" s="5" t="inlineStr">
+        <is>
+          <t>Conduct thorough investigation of all flagged transactions and activities. Enhance internal controls and fraud detection systems. Consider external audit.</t>
+        </is>
+      </c>
+      <c r="F17" s="5" t="inlineStr">
+        <is>
+          <t>7-14 days</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="inlineStr">
-        <is>
-          <t>TCB</t>
-        </is>
-      </c>
-      <c r="B18" s="3" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C18" s="3" t="inlineStr">
-        <is>
-          <t>Anomaly Detection</t>
-        </is>
-      </c>
-      <c r="D18" s="3" t="inlineStr">
-        <is>
-          <t>No significant anomalies</t>
-        </is>
-      </c>
-      <c r="E18" s="3" t="inlineStr">
-        <is>
-          <t>Continue robust monitoring and detection systems. Regularly update detection algorithms and thresholds.</t>
-        </is>
-      </c>
-      <c r="F18" s="3" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
+      <c r="A18" s="5" t="inlineStr">
+        <is>
+          <t>VPB</t>
+        </is>
+      </c>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>Liquidity Risk</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="inlineStr">
+        <is>
+          <t>Critical liquidity concerns</t>
+        </is>
+      </c>
+      <c r="E18" s="5" t="inlineStr">
+        <is>
+          <t>Immediately improve liquidity position by increasing liquid assets, reducing loan-to-deposit ratio, and establishing contingency funding plans. Consider asset sales if necessary.</t>
+        </is>
+      </c>
+      <c r="F18" s="5" t="inlineStr">
+        <is>
+          <t>Immediate</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>VCB</t>
+          <t>ACB</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1841,7 +1841,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>VCB</t>
+          <t>BIDV</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1851,17 +1851,17 @@
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>Anomaly Detection</t>
+          <t>Credit Risk</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>No significant anomalies</t>
+          <t>Strong credit risk management</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>Continue robust monitoring and detection systems. Regularly update detection algorithms and thresholds.</t>
+          <t>Continue existing practices. Share best practices with other institutions. Consider slight expansion within risk appetite.</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
@@ -1873,7 +1873,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>VPB</t>
+          <t>CTG</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1905,263 +1905,263 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
+          <t>EIB</t>
+        </is>
+      </c>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>Credit Risk</t>
+        </is>
+      </c>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>Strong credit risk management</t>
+        </is>
+      </c>
+      <c r="E22" s="3" t="inlineStr">
+        <is>
+          <t>Continue existing practices. Share best practices with other institutions. Consider slight expansion within risk appetite.</t>
+        </is>
+      </c>
+      <c r="F22" s="3" t="inlineStr">
+        <is>
+          <t>Ongoing</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>EIB</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>Anomaly Detection</t>
+        </is>
+      </c>
+      <c r="D23" s="3" t="inlineStr">
+        <is>
+          <t>No significant anomalies</t>
+        </is>
+      </c>
+      <c r="E23" s="3" t="inlineStr">
+        <is>
+          <t>Continue robust monitoring and detection systems. Regularly update detection algorithms and thresholds.</t>
+        </is>
+      </c>
+      <c r="F23" s="3" t="inlineStr">
+        <is>
+          <t>Ongoing</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>HDB</t>
+        </is>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>Credit Risk</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>Strong credit risk management</t>
+        </is>
+      </c>
+      <c r="E24" s="3" t="inlineStr">
+        <is>
+          <t>Continue existing practices. Share best practices with other institutions. Consider slight expansion within risk appetite.</t>
+        </is>
+      </c>
+      <c r="F24" s="3" t="inlineStr">
+        <is>
+          <t>Ongoing</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
+        <is>
+          <t>MBB</t>
+        </is>
+      </c>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>Credit Risk</t>
+        </is>
+      </c>
+      <c r="D25" s="3" t="inlineStr">
+        <is>
+          <t>Strong credit risk management</t>
+        </is>
+      </c>
+      <c r="E25" s="3" t="inlineStr">
+        <is>
+          <t>Continue existing practices. Share best practices with other institutions. Consider slight expansion within risk appetite.</t>
+        </is>
+      </c>
+      <c r="F25" s="3" t="inlineStr">
+        <is>
+          <t>Ongoing</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="inlineStr">
+        <is>
+          <t>STB</t>
+        </is>
+      </c>
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="inlineStr">
+        <is>
+          <t>Credit Risk</t>
+        </is>
+      </c>
+      <c r="D26" s="3" t="inlineStr">
+        <is>
+          <t>Strong credit risk management</t>
+        </is>
+      </c>
+      <c r="E26" s="3" t="inlineStr">
+        <is>
+          <t>Continue existing practices. Share best practices with other institutions. Consider slight expansion within risk appetite.</t>
+        </is>
+      </c>
+      <c r="F26" s="3" t="inlineStr">
+        <is>
+          <t>Ongoing</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="inlineStr">
+        <is>
+          <t>TCB</t>
+        </is>
+      </c>
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="inlineStr">
+        <is>
+          <t>Credit Risk</t>
+        </is>
+      </c>
+      <c r="D27" s="3" t="inlineStr">
+        <is>
+          <t>Strong credit risk management</t>
+        </is>
+      </c>
+      <c r="E27" s="3" t="inlineStr">
+        <is>
+          <t>Continue existing practices. Share best practices with other institutions. Consider slight expansion within risk appetite.</t>
+        </is>
+      </c>
+      <c r="F27" s="3" t="inlineStr">
+        <is>
+          <t>Ongoing</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="inlineStr">
+        <is>
+          <t>VCB</t>
+        </is>
+      </c>
+      <c r="B28" s="3" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="C28" s="3" t="inlineStr">
+        <is>
+          <t>Credit Risk</t>
+        </is>
+      </c>
+      <c r="D28" s="3" t="inlineStr">
+        <is>
+          <t>Strong credit risk management</t>
+        </is>
+      </c>
+      <c r="E28" s="3" t="inlineStr">
+        <is>
+          <t>Continue existing practices. Share best practices with other institutions. Consider slight expansion within risk appetite.</t>
+        </is>
+      </c>
+      <c r="F28" s="3" t="inlineStr">
+        <is>
+          <t>Ongoing</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="inlineStr">
+        <is>
           <t>VPB</t>
         </is>
       </c>
-      <c r="B22" s="3" t="inlineStr">
+      <c r="B29" s="3" t="inlineStr">
         <is>
           <t>LOW</t>
         </is>
       </c>
-      <c r="C22" s="3" t="inlineStr">
-        <is>
-          <t>Anomaly Detection</t>
-        </is>
-      </c>
-      <c r="D22" s="3" t="inlineStr">
-        <is>
-          <t>No significant anomalies</t>
-        </is>
-      </c>
-      <c r="E22" s="3" t="inlineStr">
-        <is>
-          <t>Continue robust monitoring and detection systems. Regularly update detection algorithms and thresholds.</t>
-        </is>
-      </c>
-      <c r="F22" s="3" t="inlineStr">
+      <c r="C29" s="3" t="inlineStr">
+        <is>
+          <t>Credit Risk</t>
+        </is>
+      </c>
+      <c r="D29" s="3" t="inlineStr">
+        <is>
+          <t>Strong credit risk management</t>
+        </is>
+      </c>
+      <c r="E29" s="3" t="inlineStr">
+        <is>
+          <t>Continue existing practices. Share best practices with other institutions. Consider slight expansion within risk appetite.</t>
+        </is>
+      </c>
+      <c r="F29" s="3" t="inlineStr">
         <is>
           <t>Ongoing</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="6" t="inlineStr">
-        <is>
-          <t>ACB</t>
-        </is>
-      </c>
-      <c r="B23" s="6" t="inlineStr">
-        <is>
-          <t>MEDIUM</t>
-        </is>
-      </c>
-      <c r="C23" s="6" t="inlineStr">
-        <is>
-          <t>Liquidity Risk</t>
-        </is>
-      </c>
-      <c r="D23" s="6" t="inlineStr">
-        <is>
-          <t>Moderate liquidity pressures</t>
-        </is>
-      </c>
-      <c r="E23" s="6" t="inlineStr">
-        <is>
-          <t>Strengthen liquidity buffers, diversify funding sources, and improve cash flow forecasting. Review and update contingency funding plan.</t>
-        </is>
-      </c>
-      <c r="F23" s="6" t="inlineStr">
-        <is>
-          <t>30-60 days</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="6" t="inlineStr">
-        <is>
-          <t>BIDV</t>
-        </is>
-      </c>
-      <c r="B24" s="6" t="inlineStr">
-        <is>
-          <t>MEDIUM</t>
-        </is>
-      </c>
-      <c r="C24" s="6" t="inlineStr">
-        <is>
-          <t>Liquidity Risk</t>
-        </is>
-      </c>
-      <c r="D24" s="6" t="inlineStr">
-        <is>
-          <t>Moderate liquidity pressures</t>
-        </is>
-      </c>
-      <c r="E24" s="6" t="inlineStr">
-        <is>
-          <t>Strengthen liquidity buffers, diversify funding sources, and improve cash flow forecasting. Review and update contingency funding plan.</t>
-        </is>
-      </c>
-      <c r="F24" s="6" t="inlineStr">
-        <is>
-          <t>30-60 days</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="6" t="inlineStr">
-        <is>
-          <t>CTG</t>
-        </is>
-      </c>
-      <c r="B25" s="6" t="inlineStr">
-        <is>
-          <t>MEDIUM</t>
-        </is>
-      </c>
-      <c r="C25" s="6" t="inlineStr">
-        <is>
-          <t>Liquidity Risk</t>
-        </is>
-      </c>
-      <c r="D25" s="6" t="inlineStr">
-        <is>
-          <t>Moderate liquidity pressures</t>
-        </is>
-      </c>
-      <c r="E25" s="6" t="inlineStr">
-        <is>
-          <t>Strengthen liquidity buffers, diversify funding sources, and improve cash flow forecasting. Review and update contingency funding plan.</t>
-        </is>
-      </c>
-      <c r="F25" s="6" t="inlineStr">
-        <is>
-          <t>30-60 days</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="6" t="inlineStr">
-        <is>
-          <t>EIB</t>
-        </is>
-      </c>
-      <c r="B26" s="6" t="inlineStr">
-        <is>
-          <t>MEDIUM</t>
-        </is>
-      </c>
-      <c r="C26" s="6" t="inlineStr">
-        <is>
-          <t>Liquidity Risk</t>
-        </is>
-      </c>
-      <c r="D26" s="6" t="inlineStr">
-        <is>
-          <t>Moderate liquidity pressures</t>
-        </is>
-      </c>
-      <c r="E26" s="6" t="inlineStr">
-        <is>
-          <t>Strengthen liquidity buffers, diversify funding sources, and improve cash flow forecasting. Review and update contingency funding plan.</t>
-        </is>
-      </c>
-      <c r="F26" s="6" t="inlineStr">
-        <is>
-          <t>30-60 days</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="6" t="inlineStr">
-        <is>
-          <t>HDB</t>
-        </is>
-      </c>
-      <c r="B27" s="6" t="inlineStr">
-        <is>
-          <t>MEDIUM</t>
-        </is>
-      </c>
-      <c r="C27" s="6" t="inlineStr">
-        <is>
-          <t>Liquidity Risk</t>
-        </is>
-      </c>
-      <c r="D27" s="6" t="inlineStr">
-        <is>
-          <t>Moderate liquidity pressures</t>
-        </is>
-      </c>
-      <c r="E27" s="6" t="inlineStr">
-        <is>
-          <t>Strengthen liquidity buffers, diversify funding sources, and improve cash flow forecasting. Review and update contingency funding plan.</t>
-        </is>
-      </c>
-      <c r="F27" s="6" t="inlineStr">
-        <is>
-          <t>30-60 days</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="6" t="inlineStr">
-        <is>
-          <t>MBB</t>
-        </is>
-      </c>
-      <c r="B28" s="6" t="inlineStr">
-        <is>
-          <t>MEDIUM</t>
-        </is>
-      </c>
-      <c r="C28" s="6" t="inlineStr">
-        <is>
-          <t>Liquidity Risk</t>
-        </is>
-      </c>
-      <c r="D28" s="6" t="inlineStr">
-        <is>
-          <t>Moderate liquidity pressures</t>
-        </is>
-      </c>
-      <c r="E28" s="6" t="inlineStr">
-        <is>
-          <t>Strengthen liquidity buffers, diversify funding sources, and improve cash flow forecasting. Review and update contingency funding plan.</t>
-        </is>
-      </c>
-      <c r="F28" s="6" t="inlineStr">
-        <is>
-          <t>30-60 days</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="6" t="inlineStr">
-        <is>
-          <t>STB</t>
-        </is>
-      </c>
-      <c r="B29" s="6" t="inlineStr">
-        <is>
-          <t>MEDIUM</t>
-        </is>
-      </c>
-      <c r="C29" s="6" t="inlineStr">
-        <is>
-          <t>Liquidity Risk</t>
-        </is>
-      </c>
-      <c r="D29" s="6" t="inlineStr">
-        <is>
-          <t>Moderate liquidity pressures</t>
-        </is>
-      </c>
-      <c r="E29" s="6" t="inlineStr">
-        <is>
-          <t>Strengthen liquidity buffers, diversify funding sources, and improve cash flow forecasting. Review and update contingency funding plan.</t>
-        </is>
-      </c>
-      <c r="F29" s="6" t="inlineStr">
-        <is>
-          <t>30-60 days</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="6" t="inlineStr">
         <is>
-          <t>VCB</t>
+          <t>ACB</t>
         </is>
       </c>
       <c r="B30" s="6" t="inlineStr">
@@ -2171,22 +2171,22 @@
       </c>
       <c r="C30" s="6" t="inlineStr">
         <is>
-          <t>Liquidity Risk</t>
+          <t>Anomaly Detection</t>
         </is>
       </c>
       <c r="D30" s="6" t="inlineStr">
         <is>
-          <t>Moderate liquidity pressures</t>
+          <t>Moderate unusual patterns identified</t>
         </is>
       </c>
       <c r="E30" s="6" t="inlineStr">
         <is>
-          <t>Strengthen liquidity buffers, diversify funding sources, and improve cash flow forecasting. Review and update contingency funding plan.</t>
+          <t>Review flagged activities, strengthen transaction monitoring, and improve exception reporting processes.</t>
         </is>
       </c>
       <c r="F30" s="6" t="inlineStr">
         <is>
-          <t>30-60 days</t>
+          <t>30 days</t>
         </is>
       </c>
     </row>
@@ -2203,22 +2203,22 @@
       </c>
       <c r="C31" s="6" t="inlineStr">
         <is>
-          <t>Liquidity Risk</t>
+          <t>Anomaly Detection</t>
         </is>
       </c>
       <c r="D31" s="6" t="inlineStr">
         <is>
-          <t>Moderate liquidity pressures</t>
+          <t>Moderate unusual patterns identified</t>
         </is>
       </c>
       <c r="E31" s="6" t="inlineStr">
         <is>
-          <t>Strengthen liquidity buffers, diversify funding sources, and improve cash flow forecasting. Review and update contingency funding plan.</t>
+          <t>Review flagged activities, strengthen transaction monitoring, and improve exception reporting processes.</t>
         </is>
       </c>
       <c r="F31" s="6" t="inlineStr">
         <is>
-          <t>30-60 days</t>
+          <t>30 days</t>
         </is>
       </c>
     </row>

</xml_diff>